<commit_message>
Changed the core architecture to split the data acquisition from the Kinect into its own project.  This will be needed in the future to allow concurrent Kinect v2 support.  This change breaks compatibility with the old settings files.  Also added the option to transmit the raw skeletons from each Kinect in addition to the merged skeletons.
</commit_message>
<xml_diff>
--- a/KinectWithVRServer/Joint Mapping.xlsx
+++ b/KinectWithVRServer/Joint Mapping.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ted\Documents\Visual Studio 2012\Projects\KVR\KinectWithVRServer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="28755" windowHeight="13065"/>
   </bookViews>
@@ -11,19 +16,16 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>OpenNI Joint</t>
   </si>
   <si>
-    <t>Kinect Joint</t>
-  </si>
-  <si>
     <t>Head</t>
   </si>
   <si>
@@ -157,13 +159,40 @@
   </si>
   <si>
     <t>Note: Joints numbers are picked to match the FAAST toolkit for interoperability.</t>
+  </si>
+  <si>
+    <t>Kinect v1 Joint</t>
+  </si>
+  <si>
+    <t>Kinect v2 Joint</t>
+  </si>
+  <si>
+    <t>Spine Shoulder</t>
+  </si>
+  <si>
+    <t>Spine Mid</t>
+  </si>
+  <si>
+    <t>Spine Base</t>
+  </si>
+  <si>
+    <t>Hand Tip Left</t>
+  </si>
+  <si>
+    <t>Hand Tip Right</t>
+  </si>
+  <si>
+    <t>Thumb Left</t>
+  </si>
+  <si>
+    <t>Thumb Right</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,11 +229,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -212,56 +244,233 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="Group 2"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3114675" y="266700"/>
+          <a:off x="5067300" y="266700"/>
           <a:ext cx="3743325" cy="3314700"/>
+          <a:chOff x="3400425" y="266700"/>
+          <a:chExt cx="3743325" cy="3314700"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="1">
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="1025" name="Picture 1"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="3400425" y="266700"/>
+            <a:ext cx="3743325" cy="3314700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
           <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
+          <a:ln w="1">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="TextBox 1"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4657724" y="466725"/>
+            <a:ext cx="1171575" cy="314325"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Kinect v1 Joints</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Group 3"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9153525" y="171450"/>
+          <a:ext cx="4124325" cy="4086225"/>
+          <a:chOff x="7600950" y="171450"/>
+          <a:chExt cx="4124325" cy="4086225"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="skeleton_overview_nui_skeleton" descr="Dn758662.skeleton_overview_nui_skeleton(en-us,IEB.10).png"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="7600950" y="171450"/>
+            <a:ext cx="4124325" cy="4086225"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="TextBox 5"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9172575" y="361950"/>
+            <a:ext cx="1171575" cy="314325"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Kinect v2 Joints</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -310,7 +519,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,9 +551,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,6 +586,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -551,306 +762,406 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="C25" t="s">
-        <v>43</v>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E21:J23"/>
+    <mergeCell ref="G21:L23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -859,24 +1170,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed the KinectBase.JointType enum to move the Neck joint to number 20 (which was previously skipped).  Also added the enum mapping to the joint mapping Excel file.
</commit_message>
<xml_diff>
--- a/KinectWithVRServer/Joint Mapping.xlsx
+++ b/KinectWithVRServer/Joint Mapping.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ted\Documents\Visual Studio 2012\Projects\KVR\KinectWithVRServer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="28755" windowHeight="13065"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="28755" windowHeight="13065" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="VRPN Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="Enum Mapping" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="85">
   <si>
     <t>OpenNI Joint</t>
   </si>
@@ -186,6 +180,96 @@
   </si>
   <si>
     <t>Thumb Right</t>
+  </si>
+  <si>
+    <t>Kinect Base</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>HipCenter</t>
+  </si>
+  <si>
+    <t>ShoulderCenter</t>
+  </si>
+  <si>
+    <t>ShoulderLeft</t>
+  </si>
+  <si>
+    <t>ElbowLeft</t>
+  </si>
+  <si>
+    <t>WristLeft</t>
+  </si>
+  <si>
+    <t>HandLeft</t>
+  </si>
+  <si>
+    <t>ShoulderRight</t>
+  </si>
+  <si>
+    <t>ElbowRight</t>
+  </si>
+  <si>
+    <t>WristRight</t>
+  </si>
+  <si>
+    <t>HandRight</t>
+  </si>
+  <si>
+    <t>HipLeft</t>
+  </si>
+  <si>
+    <t>KneeLeft</t>
+  </si>
+  <si>
+    <t>AnkleLeft</t>
+  </si>
+  <si>
+    <t>FootLeft</t>
+  </si>
+  <si>
+    <t>HipRight</t>
+  </si>
+  <si>
+    <t>KneeRight</t>
+  </si>
+  <si>
+    <t>AnkleRight</t>
+  </si>
+  <si>
+    <t>FootRight</t>
+  </si>
+  <si>
+    <t>HandTipLeft</t>
+  </si>
+  <si>
+    <t>ThumbLeft</t>
+  </si>
+  <si>
+    <t>HandTipRight</t>
+  </si>
+  <si>
+    <t>ThumbRight</t>
+  </si>
+  <si>
+    <t>Alt Name</t>
+  </si>
+  <si>
+    <t>SpineShoulder</t>
+  </si>
+  <si>
+    <t>SpineBase</t>
+  </si>
+  <si>
+    <t>SpineMid</t>
+  </si>
+  <si>
+    <t>Kinect v1</t>
   </si>
 </sst>
 </file>
@@ -209,12 +293,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -229,15 +319,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,6 +573,227 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6591300" y="457200"/>
+          <a:ext cx="3743325" cy="3314700"/>
+          <a:chOff x="3400425" y="266700"/>
+          <a:chExt cx="3743325" cy="3314700"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="Picture 1"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="3400425" y="266700"/>
+            <a:ext cx="3743325" cy="3314700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="1">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="TextBox 3"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4657724" y="466725"/>
+            <a:ext cx="1171575" cy="314325"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Kinect v1 Joints</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="5" name="Group 4"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10677525" y="171450"/>
+          <a:ext cx="4124325" cy="4276725"/>
+          <a:chOff x="7600950" y="171450"/>
+          <a:chExt cx="4124325" cy="4086225"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="6" name="skeleton_overview_nui_skeleton" descr="Dn758662.skeleton_overview_nui_skeleton(en-us,IEB.10).png"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="7600950" y="171450"/>
+            <a:ext cx="4124325" cy="4086225"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="TextBox 6"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9172575" y="361950"/>
+            <a:ext cx="1171575" cy="314325"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Kinect v2 Joints</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -519,7 +837,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,7 +872,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -765,7 +1083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1052,16 +1370,16 @@
       <c r="D21" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1076,14 +1394,14 @@
       <c r="D22" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1098,14 +1416,14 @@
       <c r="D23" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1171,24 +1489,583 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="5">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="5">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="5">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="5">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="5">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="5">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="5">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="5">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="5">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="5">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="5">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="5">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="5">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="5">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="5">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="5">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="5">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="5">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="5">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="5">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="5">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="5">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="5">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="5">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="5">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="5">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="5">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="5">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="5">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22">
+        <v>19</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="5">
+        <v>20</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="5">
+        <v>21</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24">
+        <v>21</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="5">
+        <v>22</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="5">
+        <v>23</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="5">
+        <v>24</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>25</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I22:N24"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the joint mapping Excel file.
</commit_message>
<xml_diff>
--- a/KinectWithVRServer/Joint Mapping.xlsx
+++ b/KinectWithVRServer/Joint Mapping.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="85">
   <si>
     <t>OpenNI Joint</t>
   </si>
@@ -326,15 +326,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1372,14 +1372,14 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1396,12 +1396,12 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1418,12 +1418,12 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1489,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,19 +1505,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1549,13 +1549,13 @@
       <c r="B3" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
@@ -1572,13 +1572,13 @@
       <c r="B4" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" t="s">
@@ -1595,19 +1595,19 @@
       <c r="B5" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>2</v>
       </c>
       <c r="F5" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>20</v>
       </c>
     </row>
@@ -1615,13 +1615,13 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>3</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>3</v>
       </c>
       <c r="F6" t="s">
@@ -1635,13 +1635,13 @@
       <c r="A7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>4</v>
       </c>
       <c r="D7" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>4</v>
       </c>
       <c r="F7" t="s">
@@ -1655,13 +1655,13 @@
       <c r="A8" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>5</v>
       </c>
       <c r="F8" t="s">
@@ -1675,13 +1675,13 @@
       <c r="A9" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>6</v>
       </c>
       <c r="F9" t="s">
@@ -1695,13 +1695,13 @@
       <c r="A10" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>7</v>
       </c>
       <c r="F10" t="s">
@@ -1715,13 +1715,13 @@
       <c r="A11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>8</v>
       </c>
       <c r="D11" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>8</v>
       </c>
       <c r="F11" t="s">
@@ -1735,13 +1735,13 @@
       <c r="A12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>9</v>
       </c>
       <c r="D12" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>9</v>
       </c>
       <c r="F12" t="s">
@@ -1755,13 +1755,13 @@
       <c r="A13" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>10</v>
       </c>
       <c r="D13" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>10</v>
       </c>
       <c r="F13" t="s">
@@ -1775,13 +1775,13 @@
       <c r="A14" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>11</v>
       </c>
       <c r="D14" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>11</v>
       </c>
       <c r="F14" t="s">
@@ -1795,13 +1795,13 @@
       <c r="A15" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>12</v>
       </c>
       <c r="D15" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="3">
         <v>12</v>
       </c>
       <c r="F15" t="s">
@@ -1815,13 +1815,13 @@
       <c r="A16" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="3">
         <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="3">
         <v>13</v>
       </c>
       <c r="F16" t="s">
@@ -1835,13 +1835,13 @@
       <c r="A17" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="3">
         <v>14</v>
       </c>
       <c r="D17" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="3">
         <v>14</v>
       </c>
       <c r="F17" t="s">
@@ -1855,13 +1855,13 @@
       <c r="A18" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="3">
         <v>15</v>
       </c>
       <c r="D18" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="3">
         <v>15</v>
       </c>
       <c r="F18" t="s">
@@ -1875,13 +1875,13 @@
       <c r="A19" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="3">
         <v>16</v>
       </c>
       <c r="D19" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="3">
         <v>16</v>
       </c>
       <c r="F19" t="s">
@@ -1895,13 +1895,13 @@
       <c r="A20" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>17</v>
       </c>
       <c r="D20" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="3">
         <v>17</v>
       </c>
       <c r="F20" t="s">
@@ -1915,13 +1915,13 @@
       <c r="A21" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <v>18</v>
       </c>
       <c r="D21" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="3">
         <v>18</v>
       </c>
       <c r="F21" t="s">
@@ -1935,13 +1935,13 @@
       <c r="A22" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="3">
         <v>19</v>
       </c>
       <c r="D22" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="3">
         <v>19</v>
       </c>
       <c r="F22" t="s">
@@ -1951,39 +1951,45 @@
         <v>19</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="5">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3">
         <v>20</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="3"/>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2</v>
+      </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>21</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="3"/>
       <c r="F24" t="s">
         <v>76</v>
       </c>
@@ -1991,21 +1997,21 @@
         <v>21</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="3">
         <v>22</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="3"/>
       <c r="F25" t="s">
         <v>77</v>
       </c>
@@ -2017,10 +2023,10 @@
       <c r="A26" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="3">
         <v>23</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="3"/>
       <c r="F26" t="s">
         <v>78</v>
       </c>
@@ -2032,29 +2038,15 @@
       <c r="A27" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="3">
         <v>24</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="3"/>
       <c r="F27" t="s">
         <v>79</v>
       </c>
       <c r="G27">
         <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="5">
-        <v>25</v>
-      </c>
-      <c r="F28" t="s">
-        <v>2</v>
-      </c>
-      <c r="G28" s="6">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>